<commit_message>
sorting strings as number in back-end
</commit_message>
<xml_diff>
--- a/Code/public/Venator_Consuting_Exported_file_text_analysis_1_1.xlsx
+++ b/Code/public/Venator_Consuting_Exported_file_text_analysis_1_1.xlsx
@@ -456,6 +456,9 @@
       <c r="C2" t="str">
         <v>550</v>
       </c>
+      <c r="D2" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E2" t="str">
         <v>K</v>
       </c>
@@ -485,6 +488,9 @@
       <c r="C3" t="str">
         <v>550</v>
       </c>
+      <c r="D3" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E3" t="str">
         <v>K</v>
       </c>
@@ -514,6 +520,9 @@
       <c r="C4" t="str">
         <v>550</v>
       </c>
+      <c r="D4" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E4" t="str">
         <v>K</v>
       </c>
@@ -543,6 +552,9 @@
       <c r="C5" t="str">
         <v>550</v>
       </c>
+      <c r="D5" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E5" t="str">
         <v>K</v>
       </c>
@@ -572,6 +584,9 @@
       <c r="C6" t="str">
         <v>550</v>
       </c>
+      <c r="D6" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E6" t="str">
         <v>K</v>
       </c>
@@ -601,6 +616,9 @@
       <c r="C7" t="str">
         <v>550</v>
       </c>
+      <c r="D7" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E7" t="str">
         <v>K</v>
       </c>
@@ -630,6 +648,9 @@
       <c r="C8" t="str">
         <v>550</v>
       </c>
+      <c r="D8" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E8" t="str">
         <v>K</v>
       </c>
@@ -659,6 +680,9 @@
       <c r="C9" t="str">
         <v>550</v>
       </c>
+      <c r="D9" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E9" t="str">
         <v>K</v>
       </c>
@@ -688,6 +712,9 @@
       <c r="C10" t="str">
         <v>550</v>
       </c>
+      <c r="D10" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E10" t="str">
         <v>K</v>
       </c>
@@ -716,6 +743,9 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <v>550</v>
+      </c>
+      <c r="D11" t="str">
+        <v>account 550</v>
       </c>
       <c r="E11" t="str">
         <v>K</v>
@@ -752,6 +782,9 @@
       <c r="C12" t="str">
         <v>550</v>
       </c>
+      <c r="D12" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E12" t="str">
         <v>K</v>
       </c>
@@ -787,6 +820,9 @@
       <c r="C13" t="str">
         <v>550</v>
       </c>
+      <c r="D13" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E13" t="str">
         <v>K</v>
       </c>
@@ -822,6 +858,9 @@
       <c r="C14" t="str">
         <v>550</v>
       </c>
+      <c r="D14" t="str">
+        <v>account 550</v>
+      </c>
       <c r="E14" t="str">
         <v>K</v>
       </c>
@@ -849,13 +888,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="str">
-        <v>fffffff</v>
+        <v/>
       </c>
       <c r="C15" t="str">
         <v>550</v>
+      </c>
+      <c r="D15" t="str">
+        <v>account 550</v>
       </c>
       <c r="E15" t="str">
         <v>K</v>
@@ -885,6 +927,9 @@
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <v>550</v>
+      </c>
+      <c r="D16" t="str">
+        <v>account 550</v>
       </c>
       <c r="E16" t="str">
         <v>K</v>

</xml_diff>